<commit_message>
Updated the main flow
</commit_message>
<xml_diff>
--- a/NWU Tech Trends Data.xlsx
+++ b/NWU Tech Trends Data.xlsx
@@ -64,6 +64,9 @@
     <x:t>contact1@techinnovators.com</x:t>
   </x:si>
   <x:si>
+    <x:t>True</x:t>
+  </x:si>
+  <x:si>
     <x:t>77af89a2-7c76-4263-a8ee-2b25541f89af</x:t>
   </x:si>
   <x:si>
@@ -199,6 +202,9 @@
     <x:t>contact16@blockchain.com</x:t>
   </x:si>
   <x:si>
+    <x:t>False</x:t>
+  </x:si>
+  <x:si>
     <x:t>66e56de0-623a-4b40-a498-0b3a77f04c16</x:t>
   </x:si>
   <x:si>
@@ -553,7 +559,7 @@
     <x:t>Creation of VR-based training programs</x:t>
   </x:si>
   <x:si>
-    <x:t>True</x:t>
+    <x:t>In Progress</x:t>
   </x:si>
   <x:si>
     <x:t>d7842f1c-4e78-4e76-b8f7-7a4b9f1d9f2e</x:t>
@@ -608,9 +614,6 @@
   </x:si>
   <x:si>
     <x:t>Scaling up the existing EdTech platform</x:t>
-  </x:si>
-  <x:si>
-    <x:t>In Progress</x:t>
   </x:si>
   <x:si>
     <x:t>c4a5b6f9-3e2f-49a5-8b7e-1d8f6c5a7b9e</x:t>
@@ -1390,691 +1393,841 @@
       <x:c r="D2" s="2">
         <x:v>44941</x:v>
       </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A3" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C3" s="1" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D3" s="2">
         <x:v>44942</x:v>
       </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A4" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B4" s="1" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C4" s="1" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D4" s="2">
         <x:v>44943</x:v>
       </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A5" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C5" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D5" s="2">
         <x:v>44944</x:v>
       </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A6" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B6" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C6" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D6" s="2">
         <x:v>44945</x:v>
       </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A7" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B7" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C7" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D7" s="2">
         <x:v>44946</x:v>
       </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A8" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C8" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D8" s="2">
         <x:v>44947</x:v>
       </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A9" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C9" s="1" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D9" s="2">
         <x:v>44948</x:v>
       </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A10" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C10" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="D10" s="2">
         <x:v>44949</x:v>
       </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A11" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C11" s="1" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D11" s="2">
         <x:v>44950</x:v>
       </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A12" s="1" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C12" s="1" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D12" s="2">
         <x:v>44951</x:v>
       </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A13" s="1" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C13" s="1" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="D13" s="2">
         <x:v>44952</x:v>
       </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A14" s="1" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C14" s="1" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="D14" s="2">
         <x:v>44953</x:v>
       </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A15" s="1" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C15" s="1" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D15" s="2">
         <x:v>44954</x:v>
       </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A16" s="1" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B16" s="1" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C16" s="1" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D16" s="2">
         <x:v>44955</x:v>
       </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A17" s="1" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B17" s="1" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C17" s="1" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D17" s="2">
         <x:v>44956</x:v>
       </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
     </x:row>
     <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A18" s="1" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B18" s="1" t="s">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C18" s="1" t="s">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D18" s="2">
         <x:v>44957</x:v>
       </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A19" s="1" t="s">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B19" s="1" t="s">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="C19" s="1" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="D19" s="2">
         <x:v>44958</x:v>
       </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A20" s="1" t="s">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B20" s="1" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C20" s="1" t="s">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="D20" s="2">
         <x:v>44959</x:v>
       </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A21" s="1" t="s">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B21" s="1" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="C21" s="1" t="s">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="D21" s="2">
         <x:v>44960</x:v>
       </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A22" s="1" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B22" s="1" t="s">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C22" s="1" t="s">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D22" s="2">
         <x:v>44961</x:v>
       </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A23" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B23" s="1" t="s">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C23" s="1" t="s">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D23" s="2">
         <x:v>44962</x:v>
       </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A24" s="1" t="s">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B24" s="1" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C24" s="1" t="s">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D24" s="2">
         <x:v>44963</x:v>
       </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A25" s="1" t="s">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B25" s="1" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C25" s="1" t="s">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="D25" s="2">
         <x:v>44964</x:v>
       </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A26" s="1" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B26" s="1" t="s">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C26" s="1" t="s">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D26" s="2">
         <x:v>44965</x:v>
       </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A27" s="1" t="s">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B27" s="1" t="s">
-        <x:v>81</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C27" s="1" t="s">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="D27" s="2">
         <x:v>44966</x:v>
       </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A28" s="1" t="s">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="B28" s="1" t="s">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C28" s="1" t="s">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="D28" s="2">
         <x:v>44967</x:v>
       </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A29" s="3" t="s">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="B29" s="1" t="s">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C29" s="1" t="s">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D29" s="2">
         <x:v>44968</x:v>
       </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A30" s="1" t="s">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="B30" s="1" t="s">
-        <x:v>90</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C30" s="1" t="s">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="D30" s="2">
         <x:v>44969</x:v>
       </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A31" s="1" t="s">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="B31" s="1" t="s">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C31" s="1" t="s">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="D31" s="2">
         <x:v>44970</x:v>
       </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A32" s="1" t="s">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="B32" s="1" t="s">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C32" s="1" t="s">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="D32" s="2">
         <x:v>44971</x:v>
       </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A33" s="1" t="s">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B33" s="1" t="s">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="C33" s="1" t="s">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="D33" s="2">
         <x:v>44972</x:v>
       </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A34" s="1" t="s">
-        <x:v>101</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B34" s="1" t="s">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C34" s="1" t="s">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="D34" s="2">
         <x:v>44973</x:v>
       </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A35" s="1" t="s">
-        <x:v>104</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="B35" s="1" t="s">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C35" s="1" t="s">
-        <x:v>106</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="D35" s="2">
         <x:v>44974</x:v>
       </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
     </x:row>
     <x:row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A36" s="1" t="s">
-        <x:v>107</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="B36" s="1" t="s">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C36" s="1" t="s">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="D36" s="2">
         <x:v>44975</x:v>
       </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A37" s="1" t="s">
-        <x:v>110</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="B37" s="1" t="s">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="C37" s="1" t="s">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="D37" s="2">
         <x:v>44976</x:v>
       </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A38" s="1" t="s">
-        <x:v>113</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="B38" s="1" t="s">
-        <x:v>114</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C38" s="1" t="s">
-        <x:v>115</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="D38" s="2">
         <x:v>44977</x:v>
       </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A39" s="1" t="s">
-        <x:v>116</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="B39" s="1" t="s">
-        <x:v>117</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="C39" s="1" t="s">
-        <x:v>118</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="D39" s="2">
         <x:v>44978</x:v>
       </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A40" s="1" t="s">
-        <x:v>119</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="B40" s="1" t="s">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C40" s="1" t="s">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="D40" s="2">
         <x:v>44979</x:v>
       </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A41" s="1" t="s">
-        <x:v>122</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="B41" s="1" t="s">
-        <x:v>123</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="C41" s="1" t="s">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="D41" s="2">
         <x:v>44980</x:v>
       </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A42" s="1" t="s">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B42" s="1" t="s">
-        <x:v>126</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C42" s="1" t="s">
-        <x:v>127</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="D42" s="2">
         <x:v>44981</x:v>
       </x:c>
+      <x:c r="E42" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A43" s="1" t="s">
-        <x:v>128</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="B43" s="1" t="s">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="C43" s="1" t="s">
-        <x:v>130</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="D43" s="2">
         <x:v>44982</x:v>
       </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A44" s="1" t="s">
-        <x:v>131</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="B44" s="1" t="s">
-        <x:v>132</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="C44" s="1" t="s">
-        <x:v>133</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="D44" s="2">
         <x:v>44983</x:v>
       </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A45" s="1" t="s">
-        <x:v>134</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="B45" s="1" t="s">
-        <x:v>135</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="C45" s="1" t="s">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="D45" s="2">
         <x:v>44984</x:v>
       </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A46" s="1" t="s">
-        <x:v>137</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="B46" s="1" t="s">
-        <x:v>138</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="C46" s="1" t="s">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D46" s="2">
         <x:v>44985</x:v>
       </x:c>
+      <x:c r="E46" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A47" s="1" t="s">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="B47" s="1" t="s">
-        <x:v>141</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="C47" s="1" t="s">
-        <x:v>142</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="D47" s="2">
         <x:v>44986</x:v>
       </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A48" s="1" t="s">
-        <x:v>143</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="B48" s="1" t="s">
-        <x:v>144</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C48" s="1" t="s">
-        <x:v>145</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D48" s="2">
         <x:v>44987</x:v>
       </x:c>
+      <x:c r="E48" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A49" s="1" t="s">
-        <x:v>146</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="B49" s="1" t="s">
-        <x:v>147</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="C49" s="1" t="s">
-        <x:v>148</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="D49" s="2">
         <x:v>44988</x:v>
       </x:c>
+      <x:c r="E49" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A50" s="1" t="s">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B50" s="1" t="s">
-        <x:v>150</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="C50" s="1" t="s">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="D50" s="2">
         <x:v>44989</x:v>
       </x:c>
+      <x:c r="E50" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A51" s="1" t="s">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B51" s="1" t="s">
-        <x:v>153</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C51" s="1" t="s">
-        <x:v>154</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="D51" s="2">
         <x:v>44990</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2109,19 +2262,19 @@
   <x:sheetData>
     <x:row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A1" s="4" t="s">
-        <x:v>155</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="B1" s="4" t="s">
-        <x:v>156</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="C1" s="4" t="s">
-        <x:v>157</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="D1" s="4" t="s">
-        <x:v>158</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="E1" s="4" t="s">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="F1" s="4" t="s">
         <x:v>0</x:v>
@@ -2132,902 +2285,938 @@
     </x:row>
     <x:row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A2" s="1" t="s">
-        <x:v>160</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
-        <x:v>161</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="C2" s="1" t="s">
-        <x:v>162</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="D2" s="2">
         <x:v>44958</x:v>
       </x:c>
       <x:c r="E2" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F2" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A3" s="1" t="s">
-        <x:v>164</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
-        <x:v>165</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="C3" s="1" t="s">
-        <x:v>166</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D3" s="2">
         <x:v>44959</x:v>
       </x:c>
       <x:c r="E3" s="1" t="s">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F3" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A4" s="1" t="s">
-        <x:v>168</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="B4" s="1" t="s">
-        <x:v>169</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C4" s="1" t="s">
-        <x:v>170</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="D4" s="2">
         <x:v>44960</x:v>
       </x:c>
       <x:c r="E4" s="1" t="s">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F4" s="1" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A5" s="1" t="s">
-        <x:v>172</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
-        <x:v>173</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="C5" s="1" t="s">
-        <x:v>174</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="D5" s="2">
         <x:v>44961</x:v>
       </x:c>
       <x:c r="E5" s="1" t="s">
-        <x:v>171</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F5" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A6" s="1" t="s">
-        <x:v>175</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="B6" s="1" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C6" s="1" t="s">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="D6" s="2">
         <x:v>44962</x:v>
       </x:c>
       <x:c r="E6" s="1" t="s">
-        <x:v>171</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F6" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A7" s="1" t="s">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="B7" s="1" t="s">
-        <x:v>179</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="C7" s="1" t="s">
-        <x:v>180</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="D7" s="2">
         <x:v>44963</x:v>
       </x:c>
       <x:c r="E7" s="1" t="s">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F7" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A8" s="1" t="s">
-        <x:v>181</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="C8" s="1" t="s">
-        <x:v>183</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="D8" s="2">
         <x:v>44964</x:v>
       </x:c>
       <x:c r="E8" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F8" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A9" s="1" t="s">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
-        <x:v>185</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="C9" s="1" t="s">
-        <x:v>186</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="D9" s="2">
         <x:v>44965</x:v>
       </x:c>
       <x:c r="E9" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F9" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A10" s="1" t="s">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
-        <x:v>188</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="C10" s="1" t="s">
-        <x:v>189</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="D10" s="2">
         <x:v>44966</x:v>
       </x:c>
       <x:c r="E10" s="1" t="s">
-        <x:v>190</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F10" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A11" s="1" t="s">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="C11" s="1" t="s">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="D11" s="2">
         <x:v>44967</x:v>
       </x:c>
       <x:c r="E11" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F11" s="1" t="s">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A12" s="1" t="s">
-        <x:v>194</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
-        <x:v>195</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="C12" s="1" t="s">
-        <x:v>196</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="D12" s="2">
         <x:v>44968</x:v>
       </x:c>
       <x:c r="E12" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F12" s="1" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A13" s="1" t="s">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
-        <x:v>198</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="C13" s="1" t="s">
-        <x:v>199</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="D13" s="2">
         <x:v>44969</x:v>
       </x:c>
       <x:c r="E13" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F13" s="1" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A14" s="1" t="s">
-        <x:v>200</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="C14" s="1" t="s">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="D14" s="2">
         <x:v>44970</x:v>
       </x:c>
       <x:c r="E14" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F14" s="1" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A15" s="1" t="s">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
-        <x:v>204</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="C15" s="1" t="s">
-        <x:v>205</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="D15" s="2">
         <x:v>44971</x:v>
       </x:c>
       <x:c r="E15" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F15" s="1" t="s">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A16" s="1" t="s">
-        <x:v>206</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="B16" s="1" t="s">
-        <x:v>207</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="C16" s="1" t="s">
-        <x:v>208</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="D16" s="2">
         <x:v>44972</x:v>
       </x:c>
       <x:c r="E16" s="1" t="s">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F16" s="1" t="s">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A17" s="1" t="s">
-        <x:v>209</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="B17" s="1" t="s">
-        <x:v>210</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="C17" s="1" t="s">
-        <x:v>211</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="D17" s="2">
         <x:v>44973</x:v>
       </x:c>
       <x:c r="E17" s="1" t="s">
-        <x:v>190</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F17" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A18" s="1" t="s">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="B18" s="1" t="s">
-        <x:v>213</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="C18" s="1" t="s">
-        <x:v>214</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="D18" s="2">
         <x:v>44974</x:v>
       </x:c>
       <x:c r="E18" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F18" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A19" s="1" t="s">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="B19" s="1" t="s">
-        <x:v>216</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="C19" s="1" t="s">
-        <x:v>217</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="D19" s="2">
         <x:v>44975</x:v>
       </x:c>
       <x:c r="E19" s="1" t="s">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F19" s="1" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A20" s="1" t="s">
-        <x:v>218</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="B20" s="1" t="s">
-        <x:v>219</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="C20" s="1" t="s">
-        <x:v>220</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="D20" s="2">
         <x:v>44976</x:v>
       </x:c>
       <x:c r="E20" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F20" s="1" t="s">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A21" s="1" t="s">
-        <x:v>221</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="B21" s="1" t="s">
-        <x:v>222</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="C21" s="1" t="s">
-        <x:v>223</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="D21" s="2">
         <x:v>44977</x:v>
       </x:c>
       <x:c r="E21" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F21" s="1" t="s">
-        <x:v>122</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A22" s="1" t="s">
-        <x:v>224</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="B22" s="1" t="s">
-        <x:v>225</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="C22" s="1" t="s">
-        <x:v>226</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="D22" s="2">
         <x:v>44978</x:v>
       </x:c>
       <x:c r="E22" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F22" s="1" t="s">
-        <x:v>107</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A23" s="1" t="s">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="B23" s="1" t="s">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="C23" s="1" t="s">
-        <x:v>229</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="D23" s="2">
         <x:v>44979</x:v>
       </x:c>
       <x:c r="E23" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F23" s="1" t="s">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A24" s="1" t="s">
-        <x:v>230</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="B24" s="1" t="s">
-        <x:v>231</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="C24" s="1" t="s">
-        <x:v>232</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="D24" s="2">
         <x:v>44980</x:v>
       </x:c>
       <x:c r="E24" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F24" s="1" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A25" s="1" t="s">
-        <x:v>233</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="B25" s="1" t="s">
-        <x:v>234</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="C25" s="1" t="s">
-        <x:v>235</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="D25" s="2">
         <x:v>44981</x:v>
       </x:c>
       <x:c r="E25" s="1" t="s">
-        <x:v>190</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F25" s="1" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A26" s="1" t="s">
-        <x:v>236</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="B26" s="1" t="s">
-        <x:v>237</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="C26" s="1" t="s">
-        <x:v>238</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="D26" s="2">
         <x:v>44982</x:v>
       </x:c>
       <x:c r="E26" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F26" s="1" t="s">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A27" s="1" t="s">
-        <x:v>239</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="B27" s="1" t="s">
-        <x:v>240</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="C27" s="1" t="s">
-        <x:v>241</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="D27" s="2">
         <x:v>44983</x:v>
       </x:c>
       <x:c r="E27" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F27" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A28" s="1" t="s">
-        <x:v>242</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="B28" s="1" t="s">
-        <x:v>243</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="C28" s="1" t="s">
-        <x:v>244</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="D28" s="2">
         <x:v>44984</x:v>
       </x:c>
       <x:c r="E28" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F28" s="1" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A29" s="1" t="s">
-        <x:v>245</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="B29" s="1" t="s">
-        <x:v>246</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="C29" s="1" t="s">
-        <x:v>247</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="D29" s="2">
         <x:v>44985</x:v>
       </x:c>
       <x:c r="E29" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F29" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A30" s="1" t="s">
-        <x:v>248</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="B30" s="1" t="s">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="C30" s="1" t="s">
-        <x:v>250</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="D30" s="2">
         <x:v>44986</x:v>
       </x:c>
       <x:c r="E30" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F30" s="1" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A31" s="1" t="s">
-        <x:v>251</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="B31" s="1" t="s">
-        <x:v>252</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="C31" s="1" t="s">
-        <x:v>253</x:v>
+        <x:v>254</x:v>
       </x:c>
       <x:c r="D31" s="2">
         <x:v>44987</x:v>
       </x:c>
       <x:c r="E31" s="1" t="s">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F31" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A32" s="1" t="s">
-        <x:v>254</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="B32" s="1" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C32" s="1" t="s">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="D32" s="2">
         <x:v>44988</x:v>
       </x:c>
       <x:c r="E32" s="1" t="s">
-        <x:v>190</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F32" s="1" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A33" s="1" t="s">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="B33" s="1" t="s">
-        <x:v>258</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="C33" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="D33" s="2">
         <x:v>44989</x:v>
       </x:c>
       <x:c r="E33" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F33" s="1" t="s">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A34" s="1" t="s">
-        <x:v>260</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="B34" s="1" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="C34" s="1" t="s">
-        <x:v>262</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="D34" s="2">
         <x:v>44990</x:v>
       </x:c>
       <x:c r="E34" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F34" s="1" t="s">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A35" s="1" t="s">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="B35" s="1" t="s">
-        <x:v>264</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="C35" s="1" t="s">
-        <x:v>265</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="D35" s="2">
         <x:v>44991</x:v>
       </x:c>
       <x:c r="E35" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F35" s="1" t="s">
-        <x:v>224</x:v>
+        <x:v>225</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A36" s="1" t="s">
-        <x:v>266</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="B36" s="1" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="C36" s="1" t="s">
-        <x:v>268</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="D36" s="2">
         <x:v>44992</x:v>
       </x:c>
       <x:c r="E36" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F36" s="1" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A37" s="1" t="s">
-        <x:v>269</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="B37" s="1" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="C37" s="1" t="s">
-        <x:v>271</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="D37" s="2">
         <x:v>44993</x:v>
       </x:c>
       <x:c r="E37" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F37" s="1" t="s">
-        <x:v>122</x:v>
+        <x:v>124</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A38" s="1" t="s">
-        <x:v>272</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="B38" s="1" t="s">
-        <x:v>273</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="C38" s="1" t="s">
-        <x:v>274</x:v>
+        <x:v>275</x:v>
       </x:c>
       <x:c r="D38" s="2">
         <x:v>44994</x:v>
       </x:c>
       <x:c r="E38" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F38" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A39" s="1" t="s">
-        <x:v>275</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="B39" s="1" t="s">
-        <x:v>276</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="C39" s="1" t="s">
-        <x:v>277</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="D39" s="2">
         <x:v>44995</x:v>
       </x:c>
       <x:c r="E39" s="1" t="s">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="F39" s="1" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A40" s="1" t="s">
-        <x:v>278</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="B40" s="1" t="s">
-        <x:v>279</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="C40" s="1" t="s">
-        <x:v>280</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="D40" s="2">
         <x:v>44996</x:v>
       </x:c>
       <x:c r="E40" s="1" t="s">
-        <x:v>190</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F40" s="1" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A41" s="1" t="s">
-        <x:v>281</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="B41" s="1" t="s">
-        <x:v>282</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="C41" s="1" t="s">
-        <x:v>283</x:v>
+        <x:v>284</x:v>
       </x:c>
       <x:c r="D41" s="2">
         <x:v>44997</x:v>
       </x:c>
       <x:c r="E41" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F41" s="1" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A42" s="1" t="s">
-        <x:v>284</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="B42" s="1" t="s">
-        <x:v>285</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="C42" s="1" t="s">
-        <x:v>286</x:v>
+        <x:v>287</x:v>
       </x:c>
       <x:c r="D42" s="2">
         <x:v>44998</x:v>
       </x:c>
       <x:c r="E42" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F42" s="1" t="s">
-        <x:v>107</x:v>
+        <x:v>109</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A43" s="1" t="s">
-        <x:v>287</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="B43" s="1" t="s">
-        <x:v>288</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="C43" s="1" t="s">
-        <x:v>289</x:v>
+        <x:v>290</x:v>
       </x:c>
       <x:c r="D43" s="2">
         <x:v>44999</x:v>
       </x:c>
       <x:c r="E43" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F43" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A44" s="1" t="s">
-        <x:v>290</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="B44" s="1" t="s">
-        <x:v>291</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="C44" s="1" t="s">
-        <x:v>292</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="D44" s="2">
         <x:v>45000</x:v>
       </x:c>
       <x:c r="E44" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F44" s="1" t="s">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A45" s="1" t="s">
-        <x:v>293</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="B45" s="1" t="s">
-        <x:v>294</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="C45" s="1" t="s">
-        <x:v>295</x:v>
+        <x:v>296</x:v>
       </x:c>
       <x:c r="D45" s="2">
         <x:v>45001</x:v>
       </x:c>
       <x:c r="E45" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F45" s="1" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A46" s="1" t="s">
-        <x:v>296</x:v>
+        <x:v>297</x:v>
       </x:c>
       <x:c r="B46" s="1" t="s">
-        <x:v>297</x:v>
+        <x:v>298</x:v>
       </x:c>
       <x:c r="C46" s="1" t="s">
-        <x:v>298</x:v>
+        <x:v>299</x:v>
       </x:c>
       <x:c r="D46" s="2">
         <x:v>45002</x:v>
       </x:c>
       <x:c r="E46" s="1" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="F46" s="1" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>